<commit_message>
Added the category feature and also added the toast feature
</commit_message>
<xml_diff>
--- a/data/menu.xlsx
+++ b/data/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programing Base\Project\Project-Nova\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A0D95F-F7A6-44A7-8EE6-846B0B203C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB50800-0AEE-481A-975D-DA5CF615C8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,66 +25,354 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="116">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Thai Soup (Double)</t>
+  </si>
+  <si>
+    <t>Soup</t>
+  </si>
+  <si>
+    <t>Thai Soup (Single)</t>
+  </si>
+  <si>
+    <t>Special Corn Soup (Double)</t>
+  </si>
+  <si>
+    <t>Special Corn Soup (Single)</t>
+  </si>
+  <si>
+    <t>Chicken Corn Soup (Double)</t>
+  </si>
+  <si>
+    <t>Chicken Corn Soup (Single)</t>
+  </si>
+  <si>
+    <t>Vegetable Corn Soup</t>
+  </si>
+  <si>
+    <t>Thai Vegetable Soup</t>
+  </si>
+  <si>
+    <t>Stim Chicken Soup</t>
+  </si>
+  <si>
+    <t>Thai Rice</t>
+  </si>
+  <si>
+    <t>Fried Rice</t>
+  </si>
+  <si>
+    <t>Chicken Rice</t>
+  </si>
+  <si>
+    <t>Vegetable Rice</t>
+  </si>
+  <si>
+    <t>Egg Rice</t>
+  </si>
+  <si>
+    <t>Thai Noodles</t>
+  </si>
+  <si>
+    <t>Noodles</t>
+  </si>
+  <si>
+    <t>Chow Mein</t>
+  </si>
+  <si>
+    <t>Vegetable Noodles</t>
+  </si>
+  <si>
+    <t>Thai Vegetable</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Chicken Vegetable</t>
+  </si>
+  <si>
+    <t>Pure Vegetable</t>
+  </si>
   <si>
     <t>Roti</t>
   </si>
   <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
     <t>Parata</t>
   </si>
   <si>
-    <t>Biryani</t>
-  </si>
-  <si>
-    <t>Breakfast</t>
-  </si>
-  <si>
-    <t>Plain Biryani</t>
-  </si>
-  <si>
-    <t>Karak Tea</t>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Daal</t>
+  </si>
+  <si>
+    <t>Paya</t>
+  </si>
+  <si>
+    <t>Beef Bhuna</t>
+  </si>
+  <si>
+    <t>Chicken Soup</t>
+  </si>
+  <si>
+    <t>Bhuna Khichdi</t>
+  </si>
+  <si>
+    <t>Chinese Vegetables</t>
+  </si>
+  <si>
+    <t>Snacks</t>
+  </si>
+  <si>
+    <t>Daal Bhaji</t>
+  </si>
+  <si>
+    <t>Singara</t>
+  </si>
+  <si>
+    <t>Samusa</t>
+  </si>
+  <si>
+    <t>Piyazu</t>
+  </si>
+  <si>
+    <t>Beguni</t>
+  </si>
+  <si>
+    <t>Mughlai</t>
+  </si>
+  <si>
+    <t>Semai</t>
+  </si>
+  <si>
+    <t>Chana</t>
+  </si>
+  <si>
+    <t>Kala Bhuna</t>
+  </si>
+  <si>
+    <t>Meals</t>
+  </si>
+  <si>
+    <t>Beef Teheri</t>
+  </si>
+  <si>
+    <t>Biriyani</t>
+  </si>
+  <si>
+    <t>Beef Biriyani</t>
+  </si>
+  <si>
+    <t>Beef Kachi Biriyani</t>
+  </si>
+  <si>
+    <t>Chicken Curry</t>
+  </si>
+  <si>
+    <t>Chicken Roast</t>
+  </si>
+  <si>
+    <t>Chicken Polaw</t>
+  </si>
+  <si>
+    <t>Chicken Biriyani</t>
+  </si>
+  <si>
+    <t>Mutton Masala</t>
+  </si>
+  <si>
+    <t>Mutton Kachi (Egg and Borhani)</t>
+  </si>
+  <si>
+    <t>Hilsha Fish Fry</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Hilsha Fish wirh Mustard</t>
+  </si>
+  <si>
+    <t>Hilsha Fish Bhuna</t>
+  </si>
+  <si>
+    <t>Shery Fish</t>
+  </si>
+  <si>
+    <t>Prawns Fish</t>
+  </si>
+  <si>
+    <t>Coral Fish</t>
+  </si>
+  <si>
+    <t>Rupchanda</t>
+  </si>
+  <si>
+    <t>Pabda Fish</t>
+  </si>
+  <si>
+    <t>Sperata Fish</t>
+  </si>
+  <si>
+    <t>Rohu Fish</t>
+  </si>
+  <si>
+    <t>Keski Fish</t>
+  </si>
+  <si>
+    <t>Koi Fish</t>
+  </si>
+  <si>
+    <t>Mola Fish</t>
+  </si>
+  <si>
+    <t>Baila Fish</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>Cold Drinks</t>
+  </si>
+  <si>
+    <t>CocaCola</t>
+  </si>
+  <si>
+    <t>Fanta</t>
+  </si>
+  <si>
+    <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Mountain Dew</t>
+  </si>
+  <si>
+    <t>Dodhi (Cup)</t>
+  </si>
+  <si>
+    <t>Sweet</t>
+  </si>
+  <si>
+    <t>Spong</t>
+  </si>
+  <si>
+    <t>Rasagolla</t>
+  </si>
+  <si>
+    <t>Lal Mohan</t>
+  </si>
+  <si>
+    <t>kalojam</t>
+  </si>
+  <si>
+    <t>Lal Cham Cham</t>
+  </si>
+  <si>
+    <t>Shada Cham Cham</t>
+  </si>
+  <si>
+    <t>Kheer Mohan</t>
+  </si>
+  <si>
+    <t>Sondesh</t>
+  </si>
+  <si>
+    <t>Dodhi Matir Cup</t>
+  </si>
+  <si>
+    <t>Water 500ml</t>
+  </si>
+  <si>
+    <t>Drinks</t>
+  </si>
+  <si>
+    <t>Water 1.5ltr</t>
+  </si>
+  <si>
+    <t>Vorta Set</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>Mix Vegetable</t>
+  </si>
+  <si>
+    <t>Borhani</t>
+  </si>
+  <si>
+    <t>Tea</t>
   </si>
   <si>
     <t>Hot Drinks</t>
   </si>
   <si>
-    <t>Daal</t>
-  </si>
-  <si>
-    <t>Vegerable</t>
-  </si>
-  <si>
-    <t>Beef Paya</t>
-  </si>
-  <si>
-    <t>Beef Bhuna</t>
-  </si>
-  <si>
-    <t>Meat</t>
-  </si>
-  <si>
-    <t>Chicken Soup</t>
-  </si>
-  <si>
-    <t>Bhuna Khichdi</t>
-  </si>
-  <si>
-    <t>Soup</t>
-  </si>
-  <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>Egg Omlet</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>category</t>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Plain Rice</t>
+  </si>
+  <si>
+    <t>Tengra Fish</t>
+  </si>
+  <si>
+    <t>Mountain Dew 1.5Ltr.</t>
+  </si>
+  <si>
+    <t>Pepsi 1.5Ltr.</t>
+  </si>
+  <si>
+    <t>7Up 1.5Ltr.</t>
+  </si>
+  <si>
+    <t>CocaCola 1.5Ltr.</t>
+  </si>
+  <si>
+    <t>Sarputi Fish</t>
+  </si>
+  <si>
+    <t>Fanta 1.5Ltr</t>
+  </si>
+  <si>
+    <t>Pepsi 2.5Ltr.</t>
+  </si>
+  <si>
+    <t>7Up 2.5Ltr.</t>
+  </si>
+  <si>
+    <t>CocaCola 2.5Ltr.</t>
+  </si>
+  <si>
+    <t>Fanta 2.5Ltr</t>
+  </si>
+  <si>
+    <t>7Up</t>
+  </si>
+  <si>
+    <t>King Fish Fry</t>
+  </si>
+  <si>
+    <t>Delivery Charge</t>
+  </si>
+  <si>
+    <t>Puri</t>
+  </si>
+  <si>
+    <t>Rasmalai</t>
   </si>
 </sst>
 </file>
@@ -419,136 +707,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
-        <v>5</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
@@ -556,13 +844,1036 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="2">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="2">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="2">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="2">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="2">
+        <v>3</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="2">
+        <v>8</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="2">
+        <v>8</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="2">
+        <v>10</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="2">
+        <v>10</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="2">
+        <v>18</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="2">
+        <v>7</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="2">
+        <v>10</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="2">
+        <v>12</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="2">
+        <v>10</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="2">
         <v>15</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="2">
+        <v>20</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="2">
+        <v>18</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="2">
+        <v>20</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="2">
+        <v>20</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="2">
+        <v>10</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="2">
+        <v>10</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="2">
+        <v>15</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" s="2">
+        <v>18</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="2">
+        <v>8</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="2">
+        <v>10</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="2">
+        <v>6</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="2">
+        <v>6</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="2">
+        <v>8</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="2">
+        <v>7</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="2">
+        <v>8</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="2">
+        <v>3</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="2">
+        <v>3</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="2">
+        <v>3</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" s="2">
+        <v>3</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="2">
+        <v>3</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" s="2">
+        <v>2</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" s="2">
+        <v>3</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="2">
+        <v>2</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" s="2">
+        <v>2</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B75" s="2">
+        <v>2</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" s="2">
+        <v>3</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" s="2">
+        <v>3</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" s="2">
+        <v>3</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="2">
+        <v>3</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B80" s="2">
+        <v>3</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81" s="2">
+        <v>1</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B82" s="2">
+        <v>2</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" s="2">
+        <v>6</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" s="2">
+        <v>5</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B85" s="2">
+        <v>2</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86" s="2">
+        <v>1</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" s="2">
+        <v>2</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88" s="2">
+        <v>1</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89" s="2">
+        <v>8</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" s="2">
+        <v>5</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" s="2">
+        <v>5</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" s="2">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93" s="2">
+        <v>5</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94" s="2">
+        <v>8</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95" s="2">
+        <v>5</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B96" s="2">
+        <v>8</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B97" s="2">
+        <v>8</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98" s="2">
+        <v>8</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99" s="2">
+        <v>8</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100" s="2">
+        <v>3</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B101" s="2">
+        <v>1</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B102" s="2">
+        <v>12</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B103" s="2">
+        <v>1</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" s="2">
+        <v>1</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B105" s="2">
+        <v>3</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>